<commit_message>
updated product_design_overview project_requirements feasibility_analysis and GUI_Design_SM_0.1
</commit_message>
<xml_diff>
--- a/evaluation/feasibility_study/Feasibility_Analysis.xlsx
+++ b/evaluation/feasibility_study/Feasibility_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcam98/Desktop/Employment/Employment_Categories/Research/CRIOS/Projects/MITgcm_solver/MITgcm-solver/evaluation/feasibility_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBF9317-CE1E-084E-B206-3A4E8A528A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8D1B93-9D43-4E44-AF9D-51452C2E6285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="19220" windowHeight="18420" activeTab="1" xr2:uid="{D88C3CD9-F38D-9947-B9A9-49F345818BAB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Weighted Scoring Matrix: Container Orchestration System</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Singularity-Compose</t>
+  </si>
+  <si>
+    <t>Apptainer</t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,8 +408,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B31CC763-C76D-D647-A226-6A541AA82D29}" name="Table13" displayName="Table13" ref="F3:F10" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="F3:F10" xr:uid="{B31CC763-C76D-D647-A226-6A541AA82D29}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B31CC763-C76D-D647-A226-6A541AA82D29}" name="Table13" displayName="Table13" ref="G3:G10" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="G3:G10" xr:uid="{B31CC763-C76D-D647-A226-6A541AA82D29}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6FC054B6-18D0-1D49-84F3-F1C4CFA3331A}" name="LEGEND" dataDxfId="0"/>
   </tableColumns>
@@ -1024,25 +1027,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDB733F-0F26-9B41-B116-D2B5C7273F54}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,13 +1059,16 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1076,11 +1082,12 @@
         <v>10</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="35" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
@@ -1093,11 +1100,11 @@
       <c r="D5">
         <v>18</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1110,11 +1117,11 @@
       <c r="D6">
         <v>17</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="35" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1127,11 +1134,11 @@
       <c r="D7">
         <v>16</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="35" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1144,11 +1151,11 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="35" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
@@ -1161,11 +1168,11 @@
       <c r="D9">
         <v>14</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1178,9 +1185,9 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1208,7 +1215,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -1222,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
@@ -1236,7 +1243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
@@ -1250,7 +1257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -1264,7 +1271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
@@ -1278,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
@@ -1292,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
@@ -1306,7 +1313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
@@ -1320,7 +1327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -1334,7 +1341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>39</v>
       </c>
@@ -1364,7 +1371,8 @@
         <f>SUM(D5:D22)</f>
         <v>123</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>